<commit_message>
add timesheet for mine
</commit_message>
<xml_diff>
--- a/Timesheet and MOM/Timesheet.xlsx
+++ b/Timesheet and MOM/Timesheet.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supatra\Documents\BubbleBeeDoc\Timesheet and MOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
@@ -19,12 +14,12 @@
     <sheet name="Week#3" sheetId="5" r:id="rId5"/>
     <sheet name="TeamMember" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
   <si>
     <t>วิธีการกรอก</t>
   </si>
@@ -332,6 +327,12 @@
   </si>
   <si>
     <t>Feasibility Study and Project Plan</t>
+  </si>
+  <si>
+    <t>ได้รับผิดชอบงานในแต่ล่ะส่วน  โดยมีการพูดภาพรวมคร่าวๆ เพื่อให้ทุกคนมองแผนงานไปในทิศทางเดียวกัน</t>
+  </si>
+  <si>
+    <t>เนื่องจากในแผนงานมีรายละเอียดมากมาย ซึ่งเมื่อทำมาแล้วอาจจะยังไม่ตรงกัน  จึงต้องมีการมารีวิวและปรับใหม่</t>
   </si>
 </sst>
 </file>
@@ -592,22 +593,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -617,40 +602,56 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,7 +714,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -748,7 +749,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -925,7 +926,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1028,42 +1029,42 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="32" t="s">
+      <c r="E8" s="47"/>
+      <c r="F8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -1260,13 +1261,13 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="35"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="19">
         <f>SUM(F10:F19)</f>
         <v>20</v>
@@ -1364,42 +1365,42 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="32" t="s">
+      <c r="E8" s="47"/>
+      <c r="F8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -1564,13 +1565,13 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="35"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="19">
         <f>SUM(F10:F15)</f>
         <v>9</v>
@@ -1668,42 +1669,42 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="32" t="s">
+      <c r="E8" s="47"/>
+      <c r="F8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="43" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -1920,13 +1921,13 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="35"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="19">
         <f>SUM(F10:F15)</f>
         <v>20.5</v>
@@ -1965,225 +1966,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="41" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="41" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="41" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="41"/>
-    <col min="5" max="5" width="19.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="41" customWidth="1"/>
-    <col min="9" max="16384" width="14.42578125" style="41"/>
+    <col min="1" max="1" width="16.85546875" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="33"/>
+    <col min="5" max="5" width="19.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="34">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="36">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="58" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+    <row r="8" spans="1:8" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="45" t="s">
+      <c r="E8" s="58"/>
+      <c r="F8" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
     </row>
     <row r="10" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="50">
+      <c r="A10" s="38">
         <v>1</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="38">
         <v>0.5</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38">
         <f>SUM(D10:E10)</f>
         <v>0.5</v>
       </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50">
+      <c r="A11" s="38">
         <v>2</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="38">
         <v>0.5</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50">
-        <f>SUM(D10:E10)</f>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38">
+        <f>SUM(D11,E11)</f>
         <v>0.5</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="50">
+      <c r="A12" s="38">
         <v>3</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="38">
         <v>0.5</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50">
-        <f>SUM(D11:E11)</f>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38">
+        <f>SUM(D12,E12)</f>
         <v>0.5</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="50">
+      <c r="A13" s="38">
         <v>4</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="38">
+        <v>3</v>
+      </c>
+      <c r="E13" s="38">
+        <v>2</v>
+      </c>
+      <c r="F13" s="38">
+        <f>SUM(D13,E13)</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="38">
+        <v>5</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="38">
         <v>0.5</v>
       </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50">
-        <f>SUM(D12:E12)</f>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38">
+        <f>SUM(D14,E14)</f>
         <v>0.5</v>
       </c>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="50">
-        <v>5</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50">
-        <f>SUM(D13:E13)</f>
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="50">
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="38">
         <f>SUM(F10:F14)</f>
-        <v>2.5</v>
-      </c>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
+        <v>7</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>